<commit_message>
LH - Updates since fork
</commit_message>
<xml_diff>
--- a/files/output/football/corners/corners.xlsx
+++ b/files/output/football/corners/corners.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,65 +447,70 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>CT</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>1HC_Res</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2HC_Res</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Tot</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>1HC</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2HC</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>1HCA</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2HCA</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>WinOverFirst</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>WinOverBoth</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>WinOverTotal</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>WinOverOne</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>WinOverTwo</t>
         </is>
@@ -517,43 +522,48 @@
           <t>West Brom</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>4,580</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>5</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>5.2</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>5.6</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>10.8</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>3.52</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>3.272</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>2.124</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>1.862</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>60</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>40</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>80</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>20</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -563,43 +573,48 @@
           <t>Rangers</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>4,582</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>5</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>4.4</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>5.4</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>9.800000000000001</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>3.998</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>3.158</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>1.334</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>2.054</v>
-      </c>
-      <c r="J3" t="n">
-        <v>80</v>
       </c>
       <c r="K3" t="n">
         <v>80</v>
       </c>
       <c r="L3" t="n">
+        <v>80</v>
+      </c>
+      <c r="M3" t="n">
         <v>100</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>60</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -609,43 +624,48 @@
           <t>PSV Eindhoven</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>4,445</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>4</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>3.75</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>4.75</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>8.5</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>3.4725</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>5.3725</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>1.7425</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>1.7275</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>75</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>25</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>75</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>25</v>
       </c>
-      <c r="N4" t="n">
+      <c r="O4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -655,872 +675,763 @@
           <t>Kilmarnock</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>4</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>4,613</t>
+        </is>
       </c>
       <c r="C5" t="n">
-        <v>4.25</v>
+        <v>5</v>
       </c>
       <c r="D5" t="n">
-        <v>4</v>
+        <v>4.4</v>
       </c>
       <c r="E5" t="n">
-        <v>8.25</v>
+        <v>3.4</v>
       </c>
       <c r="F5" t="n">
-        <v>2.04</v>
+        <v>7.800000000000001</v>
       </c>
       <c r="G5" t="n">
-        <v>2.645</v>
+        <v>2.216</v>
       </c>
       <c r="H5" t="n">
-        <v>2.1025</v>
+        <v>2.669999999999999</v>
       </c>
       <c r="I5" t="n">
-        <v>2.36</v>
+        <v>2.098</v>
       </c>
       <c r="J5" t="n">
-        <v>75</v>
+        <v>2.318000000000001</v>
       </c>
       <c r="K5" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="L5" t="n">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="M5" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="N5" t="n">
+        <v>60</v>
+      </c>
+      <c r="O5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Manchester United</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
+          <t>Burnley</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>4,559</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>4</v>
       </c>
-      <c r="C6" t="n">
-        <v>2.75</v>
-      </c>
       <c r="D6" t="n">
-        <v>4.75</v>
+        <v>3.75</v>
       </c>
       <c r="E6" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="F6" t="n">
         <v>7.5</v>
       </c>
-      <c r="F6" t="n">
-        <v>2.1275</v>
-      </c>
       <c r="G6" t="n">
-        <v>3.04</v>
+        <v>3.3525</v>
       </c>
       <c r="H6" t="n">
-        <v>1.715</v>
+        <v>3.24</v>
       </c>
       <c r="I6" t="n">
-        <v>2.09</v>
+        <v>0.9675</v>
       </c>
       <c r="J6" t="n">
+        <v>1.405</v>
+      </c>
+      <c r="K6" t="n">
+        <v>100</v>
+      </c>
+      <c r="L6" t="n">
+        <v>75</v>
+      </c>
+      <c r="M6" t="n">
+        <v>75</v>
+      </c>
+      <c r="N6" t="n">
         <v>50</v>
       </c>
-      <c r="K6" t="n">
-        <v>50</v>
-      </c>
-      <c r="L6" t="n">
-        <v>50</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="n">
+      <c r="O6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Burnley</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
+          <t>Luton</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>4,551</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
         <v>4</v>
       </c>
-      <c r="C7" t="n">
-        <v>3.75</v>
-      </c>
       <c r="D7" t="n">
-        <v>3.75</v>
+        <v>3</v>
       </c>
       <c r="E7" t="n">
-        <v>7.5</v>
+        <v>4.25</v>
       </c>
       <c r="F7" t="n">
-        <v>3.3525</v>
+        <v>7.25</v>
       </c>
       <c r="G7" t="n">
-        <v>3.24</v>
+        <v>3.0025</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9675</v>
+        <v>4.13</v>
       </c>
       <c r="I7" t="n">
-        <v>1.405</v>
+        <v>1.635</v>
       </c>
       <c r="J7" t="n">
-        <v>100</v>
+        <v>2.925</v>
       </c>
       <c r="K7" t="n">
+        <v>50</v>
+      </c>
+      <c r="L7" t="n">
+        <v>25</v>
+      </c>
+      <c r="M7" t="n">
         <v>75</v>
       </c>
-      <c r="L7" t="n">
+      <c r="N7" t="n">
         <v>75</v>
       </c>
-      <c r="M7" t="n">
-        <v>50</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0</v>
+      <c r="O7" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Luton</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>4</v>
+          <t>Manchester United</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>4,605</t>
+        </is>
       </c>
       <c r="C8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D8" t="n">
-        <v>4.25</v>
+        <v>2.8</v>
       </c>
       <c r="E8" t="n">
-        <v>7.25</v>
+        <v>4.2</v>
       </c>
       <c r="F8" t="n">
-        <v>3.0025</v>
+        <v>7</v>
       </c>
       <c r="G8" t="n">
-        <v>4.13</v>
+        <v>2.164</v>
       </c>
       <c r="H8" t="n">
-        <v>1.635</v>
+        <v>3.078</v>
       </c>
       <c r="I8" t="n">
-        <v>2.925</v>
+        <v>1.664</v>
       </c>
       <c r="J8" t="n">
-        <v>50</v>
+        <v>2.042</v>
       </c>
       <c r="K8" t="n">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="L8" t="n">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="M8" t="n">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="N8" t="n">
-        <v>25</v>
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>KVC Westerlo</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>5</v>
+          <t>Bristol City</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>4,558</t>
+        </is>
       </c>
       <c r="C9" t="n">
-        <v>2.4</v>
+        <v>4</v>
       </c>
       <c r="D9" t="n">
-        <v>4.4</v>
+        <v>2.5</v>
       </c>
       <c r="E9" t="n">
-        <v>6.800000000000001</v>
+        <v>4.25</v>
       </c>
       <c r="F9" t="n">
-        <v>3.28</v>
+        <v>6.75</v>
       </c>
       <c r="G9" t="n">
-        <v>4.05</v>
+        <v>3.19</v>
       </c>
       <c r="H9" t="n">
-        <v>2.588</v>
+        <v>2.8125</v>
       </c>
       <c r="I9" t="n">
-        <v>3.154</v>
+        <v>1.615</v>
       </c>
       <c r="J9" t="n">
-        <v>60</v>
+        <v>2.2425</v>
       </c>
       <c r="K9" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="L9" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="M9" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="N9" t="n">
-        <v>20</v>
+        <v>50</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Bristol City</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
+          <t>ST Johnstone</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>4,612</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
         <v>4</v>
       </c>
-      <c r="C10" t="n">
-        <v>2.5</v>
-      </c>
       <c r="D10" t="n">
-        <v>4.25</v>
+        <v>3.25</v>
       </c>
       <c r="E10" t="n">
-        <v>6.75</v>
+        <v>3.25</v>
       </c>
       <c r="F10" t="n">
-        <v>3.19</v>
+        <v>6.5</v>
       </c>
       <c r="G10" t="n">
-        <v>2.8125</v>
+        <v>2.6275</v>
       </c>
       <c r="H10" t="n">
-        <v>1.615</v>
+        <v>2.71</v>
       </c>
       <c r="I10" t="n">
-        <v>2.2425</v>
+        <v>3.5575</v>
       </c>
       <c r="J10" t="n">
-        <v>50</v>
+        <v>3.005</v>
       </c>
       <c r="K10" t="n">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="L10" t="n">
         <v>50</v>
       </c>
       <c r="M10" t="n">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="N10" t="n">
+        <v>100</v>
+      </c>
+      <c r="O10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Aston Villa</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
+          <t>Portsmouth</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>4,579</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
         <v>5</v>
       </c>
-      <c r="C11" t="n">
-        <v>2.4</v>
-      </c>
       <c r="D11" t="n">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="E11" t="n">
-        <v>6.6</v>
+        <v>2.8</v>
       </c>
       <c r="F11" t="n">
-        <v>2.854</v>
+        <v>6.4</v>
       </c>
       <c r="G11" t="n">
-        <v>5.191999999999999</v>
+        <v>5.312</v>
       </c>
       <c r="H11" t="n">
-        <v>1.546</v>
+        <v>2.936</v>
       </c>
       <c r="I11" t="n">
-        <v>1.582</v>
+        <v>2.106</v>
       </c>
       <c r="J11" t="n">
-        <v>80</v>
+        <v>2.74</v>
       </c>
       <c r="K11" t="n">
+        <v>100</v>
+      </c>
+      <c r="L11" t="n">
+        <v>40</v>
+      </c>
+      <c r="M11" t="n">
         <v>60</v>
       </c>
-      <c r="L11" t="n">
-        <v>60</v>
-      </c>
-      <c r="M11" t="n">
-        <v>80</v>
-      </c>
       <c r="N11" t="n">
-        <v>20</v>
+        <v>40</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Tottenham</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
+          <t>Sunderland</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>4,576</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
         <v>6</v>
       </c>
-      <c r="C12" t="n">
-        <v>2.166666666666667</v>
-      </c>
       <c r="D12" t="n">
-        <v>4.333333333333333</v>
+        <v>3.666666666666667</v>
       </c>
       <c r="E12" t="n">
-        <v>6.5</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="F12" t="n">
-        <v>4.680000000000001</v>
+        <v>6</v>
       </c>
       <c r="G12" t="n">
-        <v>3.773333333333333</v>
+        <v>3.148333333333333</v>
       </c>
       <c r="H12" t="n">
-        <v>3.491666666666667</v>
+        <v>2.701666666666667</v>
       </c>
       <c r="I12" t="n">
-        <v>2.556666666666667</v>
+        <v>2.43</v>
       </c>
       <c r="J12" t="n">
+        <v>1.766666666666667</v>
+      </c>
+      <c r="K12" t="n">
+        <v>100</v>
+      </c>
+      <c r="L12" t="n">
         <v>50</v>
-      </c>
-      <c r="K12" t="n">
-        <v>50</v>
-      </c>
-      <c r="L12" t="n">
-        <v>83.33333333333334</v>
       </c>
       <c r="M12" t="n">
         <v>66.66666666666666</v>
       </c>
       <c r="N12" t="n">
-        <v>16.66666666666666</v>
+        <v>83.33333333333334</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Portsmouth</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>5</v>
+          <t>Bournemouth</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>4,573</t>
+        </is>
       </c>
       <c r="C13" t="n">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="D13" t="n">
-        <v>2.8</v>
+        <v>3.25</v>
       </c>
       <c r="E13" t="n">
-        <v>6.4</v>
+        <v>2.5</v>
       </c>
       <c r="F13" t="n">
-        <v>5.312</v>
+        <v>5.75</v>
       </c>
       <c r="G13" t="n">
-        <v>2.936</v>
+        <v>2.525</v>
       </c>
       <c r="H13" t="n">
-        <v>2.106</v>
+        <v>3.815</v>
       </c>
       <c r="I13" t="n">
-        <v>2.74</v>
+        <v>2.465</v>
       </c>
       <c r="J13" t="n">
-        <v>100</v>
+        <v>2.7425</v>
       </c>
       <c r="K13" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="L13" t="n">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="M13" t="n">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="N13" t="n">
+        <v>25</v>
+      </c>
+      <c r="O13" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Sunderland</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>6</v>
+          <t>Sheffield Utd</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>4,589</t>
+        </is>
       </c>
       <c r="C14" t="n">
-        <v>3.666666666666667</v>
+        <v>7</v>
       </c>
       <c r="D14" t="n">
-        <v>2.333333333333333</v>
+        <v>3</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>2.428571428571428</v>
       </c>
       <c r="F14" t="n">
-        <v>3.148333333333333</v>
+        <v>5.428571428571429</v>
       </c>
       <c r="G14" t="n">
-        <v>2.701666666666667</v>
+        <v>2.862857142857143</v>
       </c>
       <c r="H14" t="n">
-        <v>2.43</v>
+        <v>3.112857142857143</v>
       </c>
       <c r="I14" t="n">
-        <v>1.766666666666667</v>
+        <v>2.124285714285715</v>
       </c>
       <c r="J14" t="n">
-        <v>100</v>
+        <v>3.02</v>
       </c>
       <c r="K14" t="n">
-        <v>50</v>
+        <v>85.71428571428571</v>
       </c>
       <c r="L14" t="n">
-        <v>66.66666666666666</v>
+        <v>71.42857142857143</v>
       </c>
       <c r="M14" t="n">
-        <v>83.33333333333334</v>
+        <v>71.42857142857143</v>
       </c>
       <c r="N14" t="n">
-        <v>0</v>
+        <v>71.42857142857143</v>
+      </c>
+      <c r="O14" t="n">
+        <v>57.14285714285714</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Sheffield Utd</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>6</v>
+          <t>Chelsea</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>4,596</t>
+        </is>
       </c>
       <c r="C15" t="n">
-        <v>3.166666666666667</v>
+        <v>4</v>
       </c>
       <c r="D15" t="n">
-        <v>2.666666666666667</v>
+        <v>3</v>
       </c>
       <c r="E15" t="n">
-        <v>5.833333333333333</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
-        <v>2.798333333333333</v>
+        <v>5</v>
       </c>
       <c r="G15" t="n">
-        <v>3.121666666666667</v>
+        <v>2.655</v>
       </c>
       <c r="H15" t="n">
-        <v>2.145</v>
+        <v>3.185</v>
       </c>
       <c r="I15" t="n">
-        <v>3.043333333333333</v>
+        <v>1.2475</v>
       </c>
       <c r="J15" t="n">
-        <v>83.33333333333334</v>
+        <v>2.075</v>
       </c>
       <c r="K15" t="n">
-        <v>83.33333333333334</v>
+        <v>75</v>
       </c>
       <c r="L15" t="n">
-        <v>83.33333333333334</v>
+        <v>25</v>
       </c>
       <c r="M15" t="n">
-        <v>66.66666666666666</v>
+        <v>50</v>
       </c>
       <c r="N15" t="n">
-        <v>66.66666666666666</v>
+        <v>50</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Bournemouth</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
+          <t>Jong Ajax</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>4,591</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
         <v>4</v>
-      </c>
-      <c r="C16" t="n">
-        <v>3.25</v>
       </c>
       <c r="D16" t="n">
         <v>2.5</v>
       </c>
       <c r="E16" t="n">
-        <v>5.75</v>
+        <v>2.5</v>
       </c>
       <c r="F16" t="n">
-        <v>2.525</v>
+        <v>5</v>
       </c>
       <c r="G16" t="n">
-        <v>3.815</v>
+        <v>2.225</v>
       </c>
       <c r="H16" t="n">
-        <v>2.465</v>
+        <v>2.905</v>
       </c>
       <c r="I16" t="n">
-        <v>2.7425</v>
+        <v>2.575</v>
       </c>
       <c r="J16" t="n">
-        <v>50</v>
+        <v>2.665</v>
       </c>
       <c r="K16" t="n">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="L16" t="n">
         <v>75</v>
       </c>
       <c r="M16" t="n">
+        <v>75</v>
+      </c>
+      <c r="N16" t="n">
+        <v>75</v>
+      </c>
+      <c r="O16" t="n">
         <v>25</v>
-      </c>
-      <c r="N16" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Norwich</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
+          <t>Stoke City</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>4,598</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>4</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F17" t="n">
         <v>5</v>
       </c>
-      <c r="C17" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="D17" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="E17" t="n">
-        <v>5.199999999999999</v>
-      </c>
-      <c r="F17" t="n">
-        <v>3</v>
-      </c>
       <c r="G17" t="n">
-        <v>2.008</v>
+        <v>2.345</v>
       </c>
       <c r="H17" t="n">
-        <v>2.288</v>
+        <v>3.0875</v>
       </c>
       <c r="I17" t="n">
-        <v>2.062</v>
+        <v>2.98</v>
       </c>
       <c r="J17" t="n">
-        <v>20</v>
+        <v>3.2925</v>
       </c>
       <c r="K17" t="n">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="L17" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="M17" t="n">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="N17" t="n">
-        <v>20</v>
+        <v>50</v>
+      </c>
+      <c r="O17" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Brentford</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
+          <t>KV Mechelen</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>4,555</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
         <v>4</v>
       </c>
-      <c r="C18" t="n">
-        <v>2.5</v>
-      </c>
       <c r="D18" t="n">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="F18" t="n">
-        <v>2.485</v>
+        <v>4.5</v>
       </c>
       <c r="G18" t="n">
-        <v>2.825</v>
+        <v>1.99</v>
       </c>
       <c r="H18" t="n">
-        <v>2.365</v>
+        <v>3.105</v>
       </c>
       <c r="I18" t="n">
-        <v>2.8025</v>
+        <v>2.6725</v>
       </c>
       <c r="J18" t="n">
-        <v>75</v>
+        <v>2.1675</v>
       </c>
       <c r="K18" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="L18" t="n">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="M18" t="n">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="N18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Coventry</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>6</v>
+          <t>Dundee</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>4,240</t>
+        </is>
       </c>
       <c r="C19" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D19" t="n">
-        <v>2.833333333333333</v>
+        <v>2.8</v>
       </c>
       <c r="E19" t="n">
-        <v>4.833333333333334</v>
+        <v>1.6</v>
       </c>
       <c r="F19" t="n">
-        <v>3.235</v>
+        <v>4.4</v>
       </c>
       <c r="G19" t="n">
-        <v>4.348333333333334</v>
+        <v>2.218</v>
       </c>
       <c r="H19" t="n">
-        <v>2.02</v>
+        <v>2.938</v>
       </c>
       <c r="I19" t="n">
-        <v>1.328333333333333</v>
+        <v>1.65</v>
       </c>
       <c r="J19" t="n">
-        <v>83.33333333333334</v>
+        <v>3.268</v>
       </c>
       <c r="K19" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="L19" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="M19" t="n">
-        <v>83.33333333333334</v>
+        <v>80</v>
       </c>
       <c r="N19" t="n">
-        <v>16.66666666666666</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>QPR</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>4</v>
-      </c>
-      <c r="C20" t="n">
-        <v>2.25</v>
-      </c>
-      <c r="D20" t="n">
-        <v>2.25</v>
-      </c>
-      <c r="E20" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="F20" t="n">
-        <v>2.745</v>
-      </c>
-      <c r="G20" t="n">
-        <v>3.365</v>
-      </c>
-      <c r="H20" t="n">
-        <v>2.37</v>
-      </c>
-      <c r="I20" t="n">
-        <v>2.415</v>
-      </c>
-      <c r="J20" t="n">
-        <v>75</v>
-      </c>
-      <c r="K20" t="n">
-        <v>25</v>
-      </c>
-      <c r="L20" t="n">
-        <v>25</v>
-      </c>
-      <c r="M20" t="n">
-        <v>25</v>
-      </c>
-      <c r="N20" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>KV Mechelen</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>4</v>
-      </c>
-      <c r="C21" t="n">
-        <v>3</v>
-      </c>
-      <c r="D21" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="E21" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="F21" t="n">
-        <v>1.99</v>
-      </c>
-      <c r="G21" t="n">
-        <v>3.105</v>
-      </c>
-      <c r="H21" t="n">
-        <v>2.6725</v>
-      </c>
-      <c r="I21" t="n">
-        <v>2.1675</v>
-      </c>
-      <c r="J21" t="n">
-        <v>25</v>
-      </c>
-      <c r="K21" t="n">
-        <v>0</v>
-      </c>
-      <c r="L21" t="n">
-        <v>25</v>
-      </c>
-      <c r="M21" t="n">
-        <v>0</v>
-      </c>
-      <c r="N21" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Dundee</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>5</v>
-      </c>
-      <c r="C22" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="D22" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="E22" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="F22" t="n">
-        <v>2.218</v>
-      </c>
-      <c r="G22" t="n">
-        <v>2.938</v>
-      </c>
-      <c r="H22" t="n">
-        <v>1.65</v>
-      </c>
-      <c r="I22" t="n">
-        <v>3.268</v>
-      </c>
-      <c r="J22" t="n">
         <v>60</v>
       </c>
-      <c r="K22" t="n">
-        <v>60</v>
-      </c>
-      <c r="L22" t="n">
-        <v>80</v>
-      </c>
-      <c r="M22" t="n">
-        <v>60</v>
-      </c>
-      <c r="N22" t="n">
+      <c r="O19" t="n">
         <v>20</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Hatayspor</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>4</v>
-      </c>
-      <c r="C23" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="D23" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="E23" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="F23" t="n">
-        <v>2.3275</v>
-      </c>
-      <c r="G23" t="n">
-        <v>2.5225</v>
-      </c>
-      <c r="H23" t="n">
-        <v>3.5875</v>
-      </c>
-      <c r="I23" t="n">
-        <v>2.72</v>
-      </c>
-      <c r="J23" t="n">
-        <v>50</v>
-      </c>
-      <c r="K23" t="n">
-        <v>50</v>
-      </c>
-      <c r="L23" t="n">
-        <v>75</v>
-      </c>
-      <c r="M23" t="n">
-        <v>75</v>
-      </c>
-      <c r="N23" t="n">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1534,7 +1445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1550,65 +1461,70 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>CT</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>1AC_Res</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2AC_Res</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Tot</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>1AC</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2AC</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>1ACA</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2ACA</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>WinOverFirst</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>WinOverBoth</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>WinOverTotal</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>WinOverOne</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>WinOverTwo</t>
         </is>
@@ -1620,43 +1536,48 @@
           <t>FC Koln - AW</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>4,499</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>3</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>4.333333333333333</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>4</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>8.333333333333332</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>3.226666666666667</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>2.88</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>2.09</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>2.873333333333333</v>
-      </c>
-      <c r="J2" t="n">
-        <v>66.66666666666666</v>
       </c>
       <c r="K2" t="n">
         <v>66.66666666666666</v>
       </c>
       <c r="L2" t="n">
-        <v>100</v>
+        <v>66.66666666666666</v>
       </c>
       <c r="M2" t="n">
         <v>100</v>
       </c>
       <c r="N2" t="n">
+        <v>100</v>
+      </c>
+      <c r="O2" t="n">
         <v>33.33333333333333</v>
       </c>
     </row>
@@ -1666,43 +1587,48 @@
           <t>Celtic - AW</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>4,581</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>5</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>3.8</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>3.6</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>7.4</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>4.304</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>3.712</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>1.07</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>2.01</v>
-      </c>
-      <c r="J3" t="n">
-        <v>60</v>
       </c>
       <c r="K3" t="n">
         <v>60</v>
       </c>
       <c r="L3" t="n">
+        <v>60</v>
+      </c>
+      <c r="M3" t="n">
         <v>80</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>100</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1712,43 +1638,48 @@
           <t>Galatasaray - AW</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>4,547</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>4</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>2.75</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>4.25</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>7</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>3.2675</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>2.76</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>2.9875</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>2.63</v>
-      </c>
-      <c r="J4" t="n">
-        <v>75</v>
       </c>
       <c r="K4" t="n">
         <v>75</v>
       </c>
       <c r="L4" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="M4" t="n">
         <v>100</v>
       </c>
       <c r="N4" t="n">
+        <v>100</v>
+      </c>
+      <c r="O4" t="n">
         <v>75</v>
       </c>
     </row>
@@ -1758,32 +1689,34 @@
           <t>Newcastle - AW</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>4,261</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>3</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>5</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>2</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>7</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>2.616666666666667</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>2.786666666666667</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>2.103333333333333</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>2.76</v>
-      </c>
-      <c r="J5" t="n">
-        <v>66.66666666666666</v>
       </c>
       <c r="K5" t="n">
         <v>66.66666666666666</v>
@@ -1792,9 +1725,12 @@
         <v>66.66666666666666</v>
       </c>
       <c r="M5" t="n">
+        <v>66.66666666666666</v>
+      </c>
+      <c r="N5" t="n">
         <v>33.33333333333333</v>
       </c>
-      <c r="N5" t="n">
+      <c r="O5" t="n">
         <v>33.33333333333333</v>
       </c>
     </row>
@@ -1804,43 +1740,48 @@
           <t>Liverpool - AW</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>4,550</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>7</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>2.857142857142857</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>4</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>6.857142857142858</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>3.66</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>3.221428571428572</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>1.607142857142857</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>1.527142857142857</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>42.85714285714285</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>28.57142857142857</v>
-      </c>
-      <c r="L6" t="n">
-        <v>57.14285714285714</v>
       </c>
       <c r="M6" t="n">
         <v>57.14285714285714</v>
       </c>
       <c r="N6" t="n">
+        <v>57.14285714285714</v>
+      </c>
+      <c r="O6" t="n">
         <v>14.28571428571428</v>
       </c>
     </row>
@@ -1850,320 +1791,202 @@
           <t>Hibernian - AW</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>4,535</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
         <v>3</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>4</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>2.666666666666667</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>6.666666666666666</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>2.38</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>3.023333333333333</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>2.213333333333333</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>3.283333333333333</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>100</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>33.33333333333333</v>
-      </c>
-      <c r="L7" t="n">
-        <v>66.66666666666666</v>
       </c>
       <c r="M7" t="n">
         <v>66.66666666666666</v>
       </c>
       <c r="N7" t="n">
+        <v>66.66666666666666</v>
+      </c>
+      <c r="O7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Rangers - AW</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
+          <t>Emmen - AW</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>4,590</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" t="n">
         <v>4</v>
       </c>
-      <c r="C8" t="n">
-        <v>3.25</v>
-      </c>
-      <c r="D8" t="n">
-        <v>3.25</v>
-      </c>
       <c r="E8" t="n">
-        <v>6.5</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="F8" t="n">
-        <v>1.72</v>
+        <v>6.333333333333334</v>
       </c>
       <c r="G8" t="n">
-        <v>4.4175</v>
+        <v>3.45</v>
       </c>
       <c r="H8" t="n">
-        <v>2.7925</v>
+        <v>3.46</v>
       </c>
       <c r="I8" t="n">
-        <v>2.4225</v>
+        <v>1.976666666666667</v>
       </c>
       <c r="J8" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="K8" t="n">
         <v>100</v>
       </c>
-      <c r="K8" t="n">
-        <v>50</v>
-      </c>
       <c r="L8" t="n">
-        <v>75</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="M8" t="n">
-        <v>50</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="N8" t="n">
-        <v>25</v>
+        <v>66.66666666666666</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Union St. Gilloise - AW</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
+          <t>Hamburger SV - AW</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>4,523</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
         <v>3</v>
       </c>
-      <c r="C9" t="n">
-        <v>1.333333333333333</v>
-      </c>
       <c r="D9" t="n">
-        <v>5</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="E9" t="n">
-        <v>6.333333333333333</v>
+        <v>3.333333333333333</v>
       </c>
       <c r="F9" t="n">
-        <v>2.37</v>
+        <v>6</v>
       </c>
       <c r="G9" t="n">
-        <v>3.376666666666667</v>
+        <v>2.3</v>
       </c>
       <c r="H9" t="n">
-        <v>1.453333333333333</v>
+        <v>2.473333333333333</v>
       </c>
       <c r="I9" t="n">
-        <v>2.453333333333333</v>
+        <v>2.253333333333333</v>
       </c>
       <c r="J9" t="n">
-        <v>66.66666666666666</v>
+        <v>3.003333333333333</v>
       </c>
       <c r="K9" t="n">
-        <v>66.66666666666666</v>
+        <v>100</v>
       </c>
       <c r="L9" t="n">
         <v>100</v>
       </c>
       <c r="M9" t="n">
-        <v>66.66666666666666</v>
+        <v>100</v>
       </c>
       <c r="N9" t="n">
+        <v>100</v>
+      </c>
+      <c r="O9" t="n">
         <v>33.33333333333333</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Hamburger SV - AW</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
+          <t>Rangers - AW</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>4,613</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" t="n">
         <v>3</v>
       </c>
-      <c r="C10" t="n">
-        <v>2.666666666666667</v>
-      </c>
-      <c r="D10" t="n">
-        <v>3.333333333333333</v>
-      </c>
       <c r="E10" t="n">
+        <v>3</v>
+      </c>
+      <c r="F10" t="n">
         <v>6</v>
       </c>
-      <c r="F10" t="n">
-        <v>2.3</v>
-      </c>
       <c r="G10" t="n">
-        <v>2.473333333333333</v>
+        <v>1.76</v>
       </c>
       <c r="H10" t="n">
-        <v>2.253333333333333</v>
+        <v>4.38</v>
       </c>
       <c r="I10" t="n">
-        <v>3.003333333333333</v>
+        <v>2.864</v>
       </c>
       <c r="J10" t="n">
-        <v>100</v>
+        <v>2.4</v>
       </c>
       <c r="K10" t="n">
         <v>100</v>
       </c>
       <c r="L10" t="n">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="M10" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="N10" t="n">
-        <v>33.33333333333333</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Servette FC - AW</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>3</v>
-      </c>
-      <c r="C11" t="n">
-        <v>2</v>
-      </c>
-      <c r="D11" t="n">
-        <v>3.333333333333333</v>
-      </c>
-      <c r="E11" t="n">
-        <v>5.333333333333334</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1.766666666666667</v>
-      </c>
-      <c r="G11" t="n">
-        <v>3.74</v>
-      </c>
-      <c r="H11" t="n">
-        <v>2.773333333333333</v>
-      </c>
-      <c r="I11" t="n">
-        <v>2.956666666666667</v>
-      </c>
-      <c r="J11" t="n">
-        <v>66.66666666666666</v>
-      </c>
-      <c r="K11" t="n">
-        <v>66.66666666666666</v>
-      </c>
-      <c r="L11" t="n">
-        <v>66.66666666666666</v>
-      </c>
-      <c r="M11" t="n">
-        <v>100</v>
-      </c>
-      <c r="N11" t="n">
-        <v>66.66666666666666</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>NEC Nijmegen - AW</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>3</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1.333333333333333</v>
-      </c>
-      <c r="D12" t="n">
-        <v>3.333333333333333</v>
-      </c>
-      <c r="E12" t="n">
-        <v>4.666666666666667</v>
-      </c>
-      <c r="F12" t="n">
-        <v>2.606666666666667</v>
-      </c>
-      <c r="G12" t="n">
-        <v>3.036666666666667</v>
-      </c>
-      <c r="H12" t="n">
-        <v>2.77</v>
-      </c>
-      <c r="I12" t="n">
-        <v>3.41</v>
-      </c>
-      <c r="J12" t="n">
-        <v>33.33333333333333</v>
-      </c>
-      <c r="K12" t="n">
-        <v>33.33333333333333</v>
-      </c>
-      <c r="L12" t="n">
-        <v>100</v>
-      </c>
-      <c r="M12" t="n">
-        <v>66.66666666666666</v>
-      </c>
-      <c r="N12" t="n">
-        <v>33.33333333333333</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Genk - AW</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>3</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="E13" t="n">
-        <v>1.333333333333333</v>
-      </c>
-      <c r="F13" t="n">
-        <v>2.653333333333333</v>
-      </c>
-      <c r="G13" t="n">
-        <v>2.926666666666667</v>
-      </c>
-      <c r="H13" t="n">
-        <v>1.79</v>
-      </c>
-      <c r="I13" t="n">
-        <v>2.36</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" t="n">
-        <v>33.33333333333333</v>
-      </c>
-      <c r="M13" t="n">
-        <v>33.33333333333333</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="O10" t="n">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2177,7 +2000,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2193,65 +2016,70 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>CT</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>1AC_Res</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2AC_Res</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Tot</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>1AC</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2AC</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>1ACA</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2ACA</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>WinOverFirst</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>WinOverBoth</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>WinOverTotal</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>WinOverOne</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>WinOverTwo</t>
         </is>
@@ -2263,43 +2091,48 @@
           <t>Celtic - AW</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>4,581</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>5</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>3.8</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>3.6</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>7.4</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>4.304</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>3.712</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>1.07</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>2.01</v>
-      </c>
-      <c r="J2" t="n">
-        <v>60</v>
       </c>
       <c r="K2" t="n">
         <v>60</v>
       </c>
       <c r="L2" t="n">
+        <v>60</v>
+      </c>
+      <c r="M2" t="n">
         <v>80</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>100</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2309,35 +2142,37 @@
           <t>KV Mechelen</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>4,513</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>5</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>3.6</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>3.8</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>7.4</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>2.048</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>2.412</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>3.431999999999999</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>3.936</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>80</v>
-      </c>
-      <c r="K3" t="n">
-        <v>60</v>
       </c>
       <c r="L3" t="n">
         <v>60</v>
@@ -2346,6 +2181,9 @@
         <v>60</v>
       </c>
       <c r="N3" t="n">
+        <v>60</v>
+      </c>
+      <c r="O3" t="n">
         <v>60</v>
       </c>
     </row>
@@ -2355,43 +2193,48 @@
           <t>Galatasaray - AW</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>4,547</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>4</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>2.75</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>4.25</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>7</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>3.2675</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>2.76</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>2.9875</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>2.63</v>
-      </c>
-      <c r="J4" t="n">
-        <v>75</v>
       </c>
       <c r="K4" t="n">
         <v>75</v>
       </c>
       <c r="L4" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="M4" t="n">
         <v>100</v>
       </c>
       <c r="N4" t="n">
+        <v>100</v>
+      </c>
+      <c r="O4" t="n">
         <v>75</v>
       </c>
     </row>
@@ -2401,43 +2244,48 @@
           <t>Liverpool - AW</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>4,550</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>7</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>2.857142857142857</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>4</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>6.857142857142858</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>3.66</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>3.221428571428572</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>1.607142857142857</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>1.527142857142857</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>42.85714285714285</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>28.57142857142857</v>
-      </c>
-      <c r="L5" t="n">
-        <v>57.14285714285714</v>
       </c>
       <c r="M5" t="n">
         <v>57.14285714285714</v>
       </c>
       <c r="N5" t="n">
+        <v>57.14285714285714</v>
+      </c>
+      <c r="O5" t="n">
         <v>14.28571428571428</v>
       </c>
     </row>
@@ -2447,43 +2295,48 @@
           <t>Sheffield Wednesday</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>4,559</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>6</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>3.166666666666667</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>3.333333333333333</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>6.5</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>3.34</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>3.168333333333333</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>2.715</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>3.285</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>83.33333333333334</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>50</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>83.33333333333334</v>
       </c>
-      <c r="M6" t="n">
+      <c r="N6" t="n">
         <v>66.66666666666666</v>
       </c>
-      <c r="N6" t="n">
+      <c r="O6" t="n">
         <v>16.66666666666666</v>
       </c>
     </row>
@@ -2493,44 +2346,49 @@
           <t>Rangers - AW</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>4</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>4,613</t>
+        </is>
       </c>
       <c r="C7" t="n">
-        <v>3.25</v>
+        <v>5</v>
       </c>
       <c r="D7" t="n">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="E7" t="n">
-        <v>6.5</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
-        <v>1.72</v>
+        <v>6</v>
       </c>
       <c r="G7" t="n">
-        <v>4.4175</v>
+        <v>1.76</v>
       </c>
       <c r="H7" t="n">
-        <v>2.7925</v>
+        <v>4.38</v>
       </c>
       <c r="I7" t="n">
-        <v>2.4225</v>
+        <v>2.864</v>
       </c>
       <c r="J7" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="K7" t="n">
         <v>100</v>
       </c>
-      <c r="K7" t="n">
-        <v>50</v>
-      </c>
       <c r="L7" t="n">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="M7" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="N7" t="n">
-        <v>25</v>
+        <v>60</v>
+      </c>
+      <c r="O7" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -2539,503 +2397,48 @@
           <t>Derby</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>4,498</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
         <v>4</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>3.5</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>1.75</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>5.25</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>2.3675</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>2.475</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>3.325</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>2.7225</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>50</v>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>50</v>
       </c>
       <c r="M8" t="n">
         <v>50</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Watford</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>4</v>
-      </c>
-      <c r="C9" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" t="n">
-        <v>3</v>
-      </c>
-      <c r="E9" t="n">
-        <v>5</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1.945</v>
-      </c>
-      <c r="G9" t="n">
-        <v>2.845</v>
-      </c>
-      <c r="H9" t="n">
-        <v>2.84</v>
-      </c>
-      <c r="I9" t="n">
-        <v>3.295</v>
-      </c>
-      <c r="J9" t="n">
-        <v>100</v>
-      </c>
-      <c r="K9" t="n">
         <v>50</v>
       </c>
-      <c r="L9" t="n">
-        <v>50</v>
-      </c>
-      <c r="M9" t="n">
-        <v>75</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Hatayspor</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>4</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="D10" t="n">
-        <v>3.25</v>
-      </c>
-      <c r="E10" t="n">
-        <v>4.75</v>
-      </c>
-      <c r="F10" t="n">
-        <v>1.8825</v>
-      </c>
-      <c r="G10" t="n">
-        <v>2.59</v>
-      </c>
-      <c r="H10" t="n">
-        <v>3.0975</v>
-      </c>
-      <c r="I10" t="n">
-        <v>3.45</v>
-      </c>
-      <c r="J10" t="n">
-        <v>75</v>
-      </c>
-      <c r="K10" t="n">
-        <v>50</v>
-      </c>
-      <c r="L10" t="n">
-        <v>75</v>
-      </c>
-      <c r="M10" t="n">
-        <v>50</v>
-      </c>
-      <c r="N10" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Wolves</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>5</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="D11" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="E11" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.8620000000000001</v>
-      </c>
-      <c r="G11" t="n">
-        <v>2.232</v>
-      </c>
-      <c r="H11" t="n">
-        <v>3.91</v>
-      </c>
-      <c r="I11" t="n">
-        <v>2.994</v>
-      </c>
-      <c r="J11" t="n">
-        <v>60</v>
-      </c>
-      <c r="K11" t="n">
-        <v>20</v>
-      </c>
-      <c r="L11" t="n">
-        <v>60</v>
-      </c>
-      <c r="M11" t="n">
-        <v>20</v>
-      </c>
-      <c r="N11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Portsmouth</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>5</v>
-      </c>
-      <c r="C12" t="n">
-        <v>2</v>
-      </c>
-      <c r="D12" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="E12" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="F12" t="n">
-        <v>1.938</v>
-      </c>
-      <c r="G12" t="n">
-        <v>1.468</v>
-      </c>
-      <c r="H12" t="n">
-        <v>3.74</v>
-      </c>
-      <c r="I12" t="n">
-        <v>3.856</v>
-      </c>
-      <c r="J12" t="n">
-        <v>100</v>
-      </c>
-      <c r="K12" t="n">
-        <v>80</v>
-      </c>
-      <c r="L12" t="n">
-        <v>100</v>
-      </c>
-      <c r="M12" t="n">
-        <v>80</v>
-      </c>
-      <c r="N12" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Ross County</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>4</v>
-      </c>
-      <c r="C13" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="D13" t="n">
-        <v>2</v>
-      </c>
-      <c r="E13" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="F13" t="n">
-        <v>1.9875</v>
-      </c>
-      <c r="G13" t="n">
-        <v>2.24</v>
-      </c>
-      <c r="H13" t="n">
-        <v>2.7625</v>
-      </c>
-      <c r="I13" t="n">
-        <v>5.5725</v>
-      </c>
-      <c r="J13" t="n">
-        <v>100</v>
-      </c>
-      <c r="K13" t="n">
-        <v>100</v>
-      </c>
-      <c r="L13" t="n">
-        <v>100</v>
-      </c>
-      <c r="M13" t="n">
-        <v>100</v>
-      </c>
-      <c r="N13" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Millwall</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>5</v>
-      </c>
-      <c r="C14" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="D14" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="E14" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="F14" t="n">
-        <v>3</v>
-      </c>
-      <c r="G14" t="n">
-        <v>2.156</v>
-      </c>
-      <c r="H14" t="n">
-        <v>2.158</v>
-      </c>
-      <c r="I14" t="n">
-        <v>3.12</v>
-      </c>
-      <c r="J14" t="n">
-        <v>100</v>
-      </c>
-      <c r="K14" t="n">
-        <v>60</v>
-      </c>
-      <c r="L14" t="n">
-        <v>60</v>
-      </c>
-      <c r="M14" t="n">
-        <v>80</v>
-      </c>
-      <c r="N14" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Motherwell</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>4</v>
-      </c>
-      <c r="C15" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" t="n">
-        <v>2</v>
-      </c>
-      <c r="E15" t="n">
-        <v>3</v>
-      </c>
-      <c r="F15" t="n">
-        <v>1.585</v>
-      </c>
-      <c r="G15" t="n">
-        <v>3.7075</v>
-      </c>
-      <c r="H15" t="n">
-        <v>4.065</v>
-      </c>
-      <c r="I15" t="n">
-        <v>3.5975</v>
-      </c>
-      <c r="J15" t="n">
-        <v>50</v>
-      </c>
-      <c r="K15" t="n">
-        <v>50</v>
-      </c>
-      <c r="L15" t="n">
-        <v>100</v>
-      </c>
-      <c r="M15" t="n">
-        <v>50</v>
-      </c>
-      <c r="N15" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>QPR</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>4</v>
-      </c>
-      <c r="C16" t="n">
-        <v>1.75</v>
-      </c>
-      <c r="D16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" t="n">
-        <v>2.75</v>
-      </c>
-      <c r="F16" t="n">
-        <v>1.8925</v>
-      </c>
-      <c r="G16" t="n">
-        <v>2.625</v>
-      </c>
-      <c r="H16" t="n">
-        <v>3.2425</v>
-      </c>
-      <c r="I16" t="n">
-        <v>4.78</v>
-      </c>
-      <c r="J16" t="n">
-        <v>50</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0</v>
-      </c>
-      <c r="N16" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Plymouth</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>4</v>
-      </c>
-      <c r="C17" t="n">
-        <v>2</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="E17" t="n">
-        <v>2.75</v>
-      </c>
-      <c r="F17" t="n">
-        <v>1.1125</v>
-      </c>
-      <c r="G17" t="n">
-        <v>1.1025</v>
-      </c>
-      <c r="H17" t="n">
-        <v>3.55</v>
-      </c>
-      <c r="I17" t="n">
-        <v>3.9</v>
-      </c>
-      <c r="J17" t="n">
-        <v>100</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0</v>
-      </c>
-      <c r="L17" t="n">
-        <v>75</v>
-      </c>
-      <c r="M17" t="n">
-        <v>75</v>
-      </c>
-      <c r="N17" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Stoke City</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>5</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D18" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="E18" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="F18" t="n">
-        <v>1.788</v>
-      </c>
-      <c r="G18" t="n">
-        <v>2.274</v>
-      </c>
-      <c r="H18" t="n">
-        <v>3.036</v>
-      </c>
-      <c r="I18" t="n">
-        <v>4.076</v>
-      </c>
-      <c r="J18" t="n">
-        <v>60</v>
-      </c>
-      <c r="K18" t="n">
-        <v>20</v>
-      </c>
-      <c r="L18" t="n">
-        <v>20</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" t="n">
+      <c r="O8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3050,7 +2453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BF2"/>
+  <dimension ref="A1:BG1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3286,318 +2689,73 @@
       </c>
       <c r="AT1" s="1" t="inlineStr">
         <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
           <t>CT</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>1HC_Res</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>2HC_Res</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>Tot</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>1HC</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>2HC</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>1HCA</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>2HCA</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>WinOverFirst</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>WinOverBoth</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>WinOverTotal</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>WinOverOne</t>
         </is>
       </c>
-      <c r="BF1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>WinOverTwo</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>4,589</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Sheffield Utd vs Leeds - AW</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>3.25</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2.69</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>3.06</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>3.38</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>1.67</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>2.88</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>0-1</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>2025-02-24</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>5.94</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>6.44</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>6.31</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>6.07</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>12.38</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>8.55</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AH2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AI2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AJ2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AK2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AL2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AM2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AN2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AO2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AP2" t="inlineStr">
-        <is>
-          <t>AWAY</t>
-        </is>
-      </c>
-      <c r="AQ2" t="inlineStr">
-        <is>
-          <t>Sheffield Utd</t>
-        </is>
-      </c>
-      <c r="AR2" t="inlineStr">
-        <is>
-          <t>Leeds - AW</t>
-        </is>
-      </c>
-      <c r="AS2" t="inlineStr">
-        <is>
-          <t>Sheffield Utd</t>
-        </is>
-      </c>
-      <c r="AT2" t="n">
-        <v>6</v>
-      </c>
-      <c r="AU2" t="n">
-        <v>3.166666666666667</v>
-      </c>
-      <c r="AV2" t="n">
-        <v>2.666666666666667</v>
-      </c>
-      <c r="AW2" t="n">
-        <v>5.833333333333333</v>
-      </c>
-      <c r="AX2" t="n">
-        <v>2.798333333333333</v>
-      </c>
-      <c r="AY2" t="n">
-        <v>3.121666666666667</v>
-      </c>
-      <c r="AZ2" t="n">
-        <v>2.145</v>
-      </c>
-      <c r="BA2" t="n">
-        <v>3.043333333333333</v>
-      </c>
-      <c r="BB2" t="n">
-        <v>83.33333333333334</v>
-      </c>
-      <c r="BC2" t="n">
-        <v>83.33333333333334</v>
-      </c>
-      <c r="BD2" t="n">
-        <v>83.33333333333334</v>
-      </c>
-      <c r="BE2" t="n">
-        <v>66.66666666666666</v>
-      </c>
-      <c r="BF2" t="n">
-        <v>66.66666666666666</v>
       </c>
     </row>
   </sheetData>
@@ -3673,34 +2831,34 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2.700916666666665</v>
+        <v>2.697190082644627</v>
       </c>
       <c r="B2" t="n">
-        <v>2.449541666666666</v>
+        <v>2.448553719008264</v>
       </c>
       <c r="C2" t="n">
-        <v>11.05695833333333</v>
+        <v>11.03789256198347</v>
       </c>
       <c r="D2" t="n">
-        <v>2.565970149253732</v>
+        <v>2.576029411764706</v>
       </c>
       <c r="E2" t="n">
-        <v>2.752014925373134</v>
+        <v>2.748308823529412</v>
       </c>
       <c r="F2" t="n">
-        <v>10.65350746268656</v>
+        <v>10.65801470588235</v>
       </c>
       <c r="G2" t="n">
-        <v>3.055833333333334</v>
+        <v>3.044008264462811</v>
       </c>
       <c r="H2" t="n">
-        <v>2.850666666666668</v>
+        <v>2.848140495867769</v>
       </c>
       <c r="I2" t="n">
-        <v>3.103955223880598</v>
+        <v>3.093823529411766</v>
       </c>
       <c r="J2" t="n">
-        <v>2.231567164179104</v>
+        <v>2.23985294117647</v>
       </c>
     </row>
   </sheetData>
@@ -3714,7 +2872,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR2"/>
+  <dimension ref="A1:AR1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3941,212 +3099,6 @@
       <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>AwayTeam</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>4,589</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Sheffield Utd vs Leeds - AW</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>3.25</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2.69</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>3.06</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>3.38</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>1.67</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>2.88</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>0-1</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>2025-02-24</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>5.94</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>6.44</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>6.31</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>6.07</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>12.38</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>8.55</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AH2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AI2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AJ2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AK2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AL2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AM2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AN2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AO2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AP2" t="inlineStr">
-        <is>
-          <t>AWAY</t>
-        </is>
-      </c>
-      <c r="AQ2" t="inlineStr">
-        <is>
-          <t>Sheffield Utd</t>
-        </is>
-      </c>
-      <c r="AR2" t="inlineStr">
-        <is>
-          <t>Leeds - AW</t>
         </is>
       </c>
     </row>
@@ -4161,7 +3113,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR241"/>
+  <dimension ref="A1:AR243"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -54979,6 +53931,450 @@
         </is>
       </c>
     </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>4,595</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>Wolves vs Fulham</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>1.92</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>2.58</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>1.42</t>
+        </is>
+      </c>
+      <c r="F242" t="inlineStr">
+        <is>
+          <t>2.42</t>
+        </is>
+      </c>
+      <c r="G242" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H242" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I242" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="J242" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K242" t="inlineStr">
+        <is>
+          <t>3.42</t>
+        </is>
+      </c>
+      <c r="L242" t="inlineStr">
+        <is>
+          <t>2.42</t>
+        </is>
+      </c>
+      <c r="M242" t="inlineStr">
+        <is>
+          <t>3.42</t>
+        </is>
+      </c>
+      <c r="N242" t="inlineStr">
+        <is>
+          <t>2.33</t>
+        </is>
+      </c>
+      <c r="O242" t="inlineStr">
+        <is>
+          <t>1-2</t>
+        </is>
+      </c>
+      <c r="P242" t="inlineStr">
+        <is>
+          <t>2025-02-25</t>
+        </is>
+      </c>
+      <c r="Q242" t="inlineStr">
+        <is>
+          <t>4.50</t>
+        </is>
+      </c>
+      <c r="R242" t="inlineStr">
+        <is>
+          <t>3.84</t>
+        </is>
+      </c>
+      <c r="S242" t="inlineStr">
+        <is>
+          <t>3.34</t>
+        </is>
+      </c>
+      <c r="T242" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="U242" t="inlineStr">
+        <is>
+          <t>8.34</t>
+        </is>
+      </c>
+      <c r="V242" t="inlineStr">
+        <is>
+          <t>11.59</t>
+        </is>
+      </c>
+      <c r="W242" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="X242" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="Y242" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="Z242" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AA242" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB242" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AC242" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AD242" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AE242" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AF242" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG242" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AH242" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AI242" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AJ242" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AK242" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AL242" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AM242" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AN242" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AO242" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP242" t="inlineStr">
+        <is>
+          <t>HOME</t>
+        </is>
+      </c>
+      <c r="AQ242" t="inlineStr">
+        <is>
+          <t>Wolves</t>
+        </is>
+      </c>
+      <c r="AR242" t="inlineStr">
+        <is>
+          <t>Fulham</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>4,601</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>Hamilton Academical vs Dunfermline - AW</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>3.17</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>2.08</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>1.83</t>
+        </is>
+      </c>
+      <c r="F243" t="inlineStr">
+        <is>
+          <t>2.08</t>
+        </is>
+      </c>
+      <c r="G243" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H243" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I243" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="J243" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="K243" t="inlineStr">
+        <is>
+          <t>2.17</t>
+        </is>
+      </c>
+      <c r="L243" t="inlineStr">
+        <is>
+          <t>2.58</t>
+        </is>
+      </c>
+      <c r="M243" t="inlineStr">
+        <is>
+          <t>3.08</t>
+        </is>
+      </c>
+      <c r="N243" t="inlineStr">
+        <is>
+          <t>2.5</t>
+        </is>
+      </c>
+      <c r="O243" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="P243" t="inlineStr">
+        <is>
+          <t>2025-02-25</t>
+        </is>
+      </c>
+      <c r="Q243" t="inlineStr">
+        <is>
+          <t>5.25</t>
+        </is>
+      </c>
+      <c r="R243" t="inlineStr">
+        <is>
+          <t>3.91</t>
+        </is>
+      </c>
+      <c r="S243" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="T243" t="inlineStr">
+        <is>
+          <t>4.16</t>
+        </is>
+      </c>
+      <c r="U243" t="inlineStr">
+        <is>
+          <t>9.16</t>
+        </is>
+      </c>
+      <c r="V243" t="inlineStr">
+        <is>
+          <t>10.33</t>
+        </is>
+      </c>
+      <c r="W243" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="X243" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="Y243" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="Z243" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AA243" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB243" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AC243" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AD243" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AE243" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AF243" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG243" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AH243" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AI243" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AJ243" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AK243" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AL243" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AM243" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AN243" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AO243" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP243" t="inlineStr">
+        <is>
+          <t>AWAY</t>
+        </is>
+      </c>
+      <c r="AQ243" t="inlineStr">
+        <is>
+          <t>Hamilton Academical</t>
+        </is>
+      </c>
+      <c r="AR243" t="inlineStr">
+        <is>
+          <t>Dunfermline - AW</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>